<commit_message>
Changes as of September 29, 2019
</commit_message>
<xml_diff>
--- a/Drug Defaults.xlsx
+++ b/Drug Defaults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\StanpumpR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BFD02CE-CBE6-4A1C-986C-C03DD30BEA0B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AF1365-0A2F-443C-B914-9D36CB419AF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1103" yWindow="1103" windowWidth="16875" windowHeight="10635" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="62">
   <si>
     <t>propofol</t>
   </si>
@@ -162,13 +162,70 @@
     <t>#008F7D</t>
   </si>
   <si>
-    <t>Awake</t>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>oxycodone</t>
+  </si>
+  <si>
+    <t>mg po</t>
+  </si>
+  <si>
+    <t>Emerge</t>
+  </si>
+  <si>
+    <t>mg,mg/hr</t>
+  </si>
+  <si>
+    <t>mg,mg/hr,mg po</t>
+  </si>
+  <si>
+    <t>mg,mg/kg/min</t>
+  </si>
+  <si>
+    <t>mg,mg/kg/hr</t>
+  </si>
+  <si>
+    <t>mcg,mcg/min</t>
+  </si>
+  <si>
+    <t>Default Units</t>
+  </si>
+  <si>
+    <t>mcg,mcg/kg,mcg/hr,mcg/kg/hr</t>
+  </si>
+  <si>
+    <t>MEAC</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Typical</t>
+  </si>
+  <si>
+    <t>mg,mg/kg,mcg/kg/min</t>
+  </si>
+  <si>
+    <t>mcg,mcg/kg,mcg/kg/min</t>
+  </si>
+  <si>
+    <t>mcg,mcg/kg,mcg/kg/hr</t>
+  </si>
+  <si>
+    <t>mg,mg/kg,mg/hr</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.00000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -204,9 +261,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -521,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBD3CBA1-6D90-4E49-BCBD-CB4D09098359}">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -533,9 +591,14 @@
     <col min="2" max="2" width="18.1328125" customWidth="1"/>
     <col min="3" max="3" width="13.9296875" customWidth="1"/>
     <col min="4" max="4" width="13.1328125" customWidth="1"/>
+    <col min="5" max="5" width="13.46484375" customWidth="1"/>
+    <col min="6" max="6" width="17.19921875" customWidth="1"/>
+    <col min="7" max="7" width="11.3984375" customWidth="1"/>
+    <col min="8" max="8" width="9.06640625" style="2" customWidth="1"/>
+    <col min="9" max="10" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -549,13 +612,31 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>28</v>
+        <v>52</v>
       </c>
       <c r="F1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="G1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I1" t="s">
+        <v>55</v>
+      </c>
+      <c r="J1" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" t="s">
+        <v>54</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -569,13 +650,31 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>58</v>
+      </c>
+      <c r="G2" t="s">
         <v>29</v>
       </c>
-      <c r="F2">
+      <c r="H2">
+        <v>2.5</v>
+      </c>
+      <c r="I2">
+        <v>4</v>
+      </c>
+      <c r="J2">
+        <v>3</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -589,13 +688,31 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>38</v>
       </c>
-      <c r="F3">
+      <c r="H3">
+        <v>0.8</v>
+      </c>
+      <c r="I3">
+        <v>2</v>
+      </c>
+      <c r="J3">
+        <v>1.2</v>
+      </c>
+      <c r="K3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="L3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -609,13 +726,31 @@
         <v>19</v>
       </c>
       <c r="E4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F4" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" t="s">
         <v>33</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H4">
+        <v>0.48</v>
+      </c>
+      <c r="I4">
+        <v>1.2</v>
+      </c>
+      <c r="J4">
+        <v>0.72</v>
+      </c>
+      <c r="K4">
+        <v>0.6</v>
+      </c>
+      <c r="L4">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -629,13 +764,31 @@
         <v>19</v>
       </c>
       <c r="E5" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" t="s">
         <v>33</v>
       </c>
-      <c r="F5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H5">
+        <v>31.2</v>
+      </c>
+      <c r="I5">
+        <v>78</v>
+      </c>
+      <c r="J5">
+        <v>46.8</v>
+      </c>
+      <c r="K5">
+        <v>39</v>
+      </c>
+      <c r="L5">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -649,13 +802,31 @@
         <v>19</v>
       </c>
       <c r="E6" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" t="s">
+        <v>60</v>
+      </c>
+      <c r="G6" t="s">
         <v>33</v>
       </c>
-      <c r="F6">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H6">
+        <v>4.48E-2</v>
+      </c>
+      <c r="I6">
+        <v>0.112</v>
+      </c>
+      <c r="J6">
+        <v>6.7199999999999996E-2</v>
+      </c>
+      <c r="K6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="L6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -669,13 +840,31 @@
         <v>20</v>
       </c>
       <c r="E7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" t="s">
+        <v>47</v>
+      </c>
+      <c r="G7" t="s">
         <v>32</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H7">
+        <v>6.4000000000000003E-3</v>
+      </c>
+      <c r="I7">
+        <v>1.6E-2</v>
+      </c>
+      <c r="J7">
+        <v>9.5999999999999992E-3</v>
+      </c>
+      <c r="K7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="L7">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>26</v>
       </c>
@@ -689,13 +878,31 @@
         <v>20</v>
       </c>
       <c r="E8" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" t="s">
         <v>39</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H8">
+        <v>0.2</v>
+      </c>
+      <c r="I8">
+        <v>0.5</v>
+      </c>
+      <c r="J8">
+        <v>0.3</v>
+      </c>
+      <c r="K8">
+        <v>0.25</v>
+      </c>
+      <c r="L8">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -709,13 +916,31 @@
         <v>20</v>
       </c>
       <c r="E9" t="s">
+        <v>15</v>
+      </c>
+      <c r="F9" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" t="s">
         <v>32</v>
       </c>
-      <c r="F9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H9">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="I9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K9">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L9">
+        <v>1.5E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -729,13 +954,31 @@
         <v>20</v>
       </c>
       <c r="E10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" t="s">
         <v>31</v>
       </c>
-      <c r="F10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H10">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I10">
+        <v>0.12</v>
+      </c>
+      <c r="J10">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="K10">
+        <v>0.06</v>
+      </c>
+      <c r="L10">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -749,13 +992,31 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
+        <v>15</v>
+      </c>
+      <c r="F11" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" t="s">
         <v>29</v>
       </c>
-      <c r="F11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H11">
+        <v>0.1</v>
+      </c>
+      <c r="I11">
+        <v>0.16</v>
+      </c>
+      <c r="J11">
+        <v>0.12</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -769,13 +1030,31 @@
         <v>19</v>
       </c>
       <c r="E12" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" t="s">
+        <v>53</v>
+      </c>
+      <c r="G12" t="s">
         <v>37</v>
       </c>
-      <c r="F12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H12">
+        <v>0.4</v>
+      </c>
+      <c r="I12">
+        <v>0.8</v>
+      </c>
+      <c r="J12">
+        <v>10</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -789,13 +1068,31 @@
         <v>20</v>
       </c>
       <c r="E13" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" t="s">
+        <v>61</v>
+      </c>
+      <c r="G13" t="s">
         <v>36</v>
       </c>
-      <c r="F13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H13">
+        <v>0.04</v>
+      </c>
+      <c r="I13">
+        <v>0.12</v>
+      </c>
+      <c r="J13">
+        <v>0.1</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0.04</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -809,13 +1106,31 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
+        <v>15</v>
+      </c>
+      <c r="F14" t="s">
+        <v>49</v>
+      </c>
+      <c r="G14" t="s">
         <v>29</v>
       </c>
-      <c r="F14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="H14">
+        <v>0.4</v>
+      </c>
+      <c r="I14">
+        <v>0.8</v>
+      </c>
+      <c r="J14">
+        <v>0.5</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -829,13 +1144,31 @@
         <v>20</v>
       </c>
       <c r="E15" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" t="s">
+        <v>47</v>
+      </c>
+      <c r="G15" t="s">
         <v>34</v>
       </c>
-      <c r="F15">
+      <c r="H15">
+        <v>0.5</v>
+      </c>
+      <c r="I15">
+        <v>1.5</v>
+      </c>
+      <c r="J15">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -849,13 +1182,31 @@
         <v>27</v>
       </c>
       <c r="E16" t="s">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>50</v>
+      </c>
+      <c r="G16" t="s">
         <v>30</v>
       </c>
-      <c r="F16">
+      <c r="H16">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="I16">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="J16">
+        <v>1.5</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>25</v>
       </c>
@@ -869,13 +1220,31 @@
         <v>41</v>
       </c>
       <c r="E17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" t="s">
         <v>35</v>
       </c>
-      <c r="F17">
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -889,10 +1258,60 @@
         <v>41</v>
       </c>
       <c r="E18" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" t="s">
         <v>42</v>
       </c>
-      <c r="F18">
-        <v>1</v>
+      <c r="H18">
+        <v>0.05</v>
+      </c>
+      <c r="I18">
+        <v>0.2</v>
+      </c>
+      <c r="J18">
+        <v>0.1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>44</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" t="s">
+        <v>45</v>
+      </c>
+      <c r="G19" t="s">
+        <v>32</v>
+      </c>
+      <c r="H19">
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="I19">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="J19">
+        <v>1.8E-3</v>
+      </c>
+      <c r="K19">
+        <v>1.5E-3</v>
+      </c>
+      <c r="L19">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update as of October 14, 2019
</commit_message>
<xml_diff>
--- a/Drug Defaults.xlsx
+++ b/Drug Defaults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\StanpumpR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AF1365-0A2F-443C-B914-9D36CB419AF1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CD71CD7-9345-428A-BEC8-90C5507E2D3B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14746" xr2:uid="{F1EDE105-E79D-43EB-8BB3-A0EECCFD5A7A}"/>
   </bookViews>
@@ -168,18 +168,12 @@
     <t>oxycodone</t>
   </si>
   <si>
-    <t>mg po</t>
-  </si>
-  <si>
     <t>Emerge</t>
   </si>
   <si>
     <t>mg,mg/hr</t>
   </si>
   <si>
-    <t>mg,mg/hr,mg po</t>
-  </si>
-  <si>
     <t>mg,mg/kg/min</t>
   </si>
   <si>
@@ -207,9 +201,6 @@
     <t>Typical</t>
   </si>
   <si>
-    <t>mg,mg/kg,mcg/kg/min</t>
-  </si>
-  <si>
     <t>mcg,mcg/kg,mcg/kg/min</t>
   </si>
   <si>
@@ -217,6 +208,15 @@
   </si>
   <si>
     <t>mg,mg/kg,mg/hr</t>
+  </si>
+  <si>
+    <t>mg,mg/kg,mcg/kg/min,mg/kg/hr</t>
+  </si>
+  <si>
+    <t>mg PO</t>
+  </si>
+  <si>
+    <t>mg,mg/kg,mg/hr,mg/kg/hr,mg PO,mg IM,mg IN</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -612,7 +612,7 @@
         <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="F1" t="s">
         <v>43</v>
@@ -621,19 +621,19 @@
         <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="I1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" t="s">
         <v>55</v>
       </c>
-      <c r="J1" t="s">
-        <v>57</v>
-      </c>
       <c r="K1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.45">
@@ -653,7 +653,7 @@
         <v>15</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G2" t="s">
         <v>29</v>
@@ -691,7 +691,7 @@
         <v>18</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="G3" t="s">
         <v>38</v>
@@ -729,7 +729,7 @@
         <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
         <v>33</v>
@@ -767,7 +767,7 @@
         <v>16</v>
       </c>
       <c r="F5" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G5" t="s">
         <v>33</v>
@@ -805,7 +805,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="G6" t="s">
         <v>33</v>
@@ -843,7 +843,7 @@
         <v>15</v>
       </c>
       <c r="F7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G7" t="s">
         <v>32</v>
@@ -881,7 +881,7 @@
         <v>15</v>
       </c>
       <c r="F8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G8" t="s">
         <v>39</v>
@@ -907,7 +907,7 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
         <v>15</v>
@@ -919,25 +919,25 @@
         <v>15</v>
       </c>
       <c r="F9" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="G9" t="s">
         <v>32</v>
       </c>
       <c r="H9">
-        <v>1.1999999999999999E-3</v>
+        <v>1.2</v>
       </c>
       <c r="I9">
-        <v>3.0000000000000001E-3</v>
+        <v>3</v>
       </c>
       <c r="J9">
-        <v>1.8E-3</v>
+        <v>1.8</v>
       </c>
       <c r="K9">
-        <v>1.5E-3</v>
+        <v>1.5</v>
       </c>
       <c r="L9">
-        <v>1.5E-3</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.45">
@@ -957,7 +957,7 @@
         <v>15</v>
       </c>
       <c r="F10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G10" t="s">
         <v>31</v>
@@ -995,7 +995,7 @@
         <v>15</v>
       </c>
       <c r="F11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G11" t="s">
         <v>29</v>
@@ -1033,7 +1033,7 @@
         <v>19</v>
       </c>
       <c r="F12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="G12" t="s">
         <v>37</v>
@@ -1071,7 +1071,7 @@
         <v>15</v>
       </c>
       <c r="F13" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G13" t="s">
         <v>36</v>
@@ -1109,7 +1109,7 @@
         <v>15</v>
       </c>
       <c r="F14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G14" t="s">
         <v>29</v>
@@ -1147,7 +1147,7 @@
         <v>15</v>
       </c>
       <c r="F15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G15" t="s">
         <v>34</v>
@@ -1185,7 +1185,7 @@
         <v>15</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
         <v>30</v>
@@ -1223,7 +1223,7 @@
         <v>16</v>
       </c>
       <c r="F17" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G17" t="s">
         <v>35</v>
@@ -1261,7 +1261,7 @@
         <v>16</v>
       </c>
       <c r="F18" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G18" t="s">
         <v>42</v>
@@ -1287,31 +1287,31 @@
         <v>44</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E19" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="F19" t="s">
-        <v>45</v>
+        <v>60</v>
       </c>
       <c r="G19" t="s">
         <v>32</v>
       </c>
       <c r="H19">
-        <v>1.1999999999999999E-3</v>
+        <v>10</v>
       </c>
       <c r="I19">
-        <v>3.0000000000000001E-3</v>
+        <v>20</v>
       </c>
       <c r="J19">
-        <v>1.8E-3</v>
+        <v>14</v>
       </c>
       <c r="K19">
-        <v>1.5E-3</v>
+        <v>12</v>
       </c>
       <c r="L19">
-        <v>1E-3</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>